<commit_message>
Update median of clusters (no mundist-f).xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/median of clusters (no mundist-f).xlsx
+++ b/migforecasting/clustering/median of clusters (no mundist-f).xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>clust</t>
   </si>
@@ -92,12 +92,18 @@
   <si>
     <t>5</t>
   </si>
+  <si>
+    <t>abs (worst - real)</t>
+  </si>
+  <si>
+    <t>wors case</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -142,17 +155,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1043,7 +1073,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>Sheet1!$AH$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1066,7 +1096,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$7</c:f>
+              <c:f>Sheet1!$AH$2:$AH$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4356,14 +4386,14 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>31297</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:rowOff>102735</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4706,13 +4736,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -4770,6 +4803,12 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="X1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4827,28 +4866,34 @@
         <v>22959.999999999902</v>
       </c>
       <c r="D2" s="2">
-        <v>5237.99999999999</v>
+        <f>X2/C2</f>
+        <v>0.22813588850174271</v>
       </c>
       <c r="E2" s="2">
         <v>22823.06667</v>
       </c>
       <c r="F2" s="2">
-        <v>16359.199999999901</v>
+        <f>Z2/C2</f>
+        <v>0.71250871080139244</v>
       </c>
       <c r="G2" s="2">
-        <v>552.99999999999898</v>
+        <f>AA2/C2</f>
+        <v>2.4085365853658596E-2</v>
       </c>
       <c r="H2" s="2">
-        <v>706400.680319999</v>
+        <f>AB2/C2</f>
+        <v>30.766580153310194</v>
       </c>
       <c r="I2" s="2">
         <v>26.5</v>
       </c>
       <c r="J2" s="2">
-        <v>58.999999999999901</v>
+        <f>AD2/C2</f>
+        <v>2.5696864111498323E-3</v>
       </c>
       <c r="K2" s="2">
-        <v>67.999999999999901</v>
+        <f>AE2/C2</f>
+        <v>2.9616724738676043E-3</v>
       </c>
       <c r="L2" s="2">
         <v>133.79999999999899</v>
@@ -4857,19 +4902,30 @@
         <v>3356.99999999999</v>
       </c>
       <c r="N2" s="2">
-        <v>6361.6199999999899</v>
+        <f>AH2/C2</f>
+        <v>0.27707404181184742</v>
       </c>
       <c r="O2" s="2">
         <v>95221.072399999903</v>
       </c>
       <c r="P2" s="2">
-        <v>4.9999999999999902</v>
+        <f>AJ2/C2</f>
+        <v>2.1777003484320609E-4</v>
       </c>
       <c r="Q2" s="2">
-        <v>1274.99999999999</v>
+        <f>AK2/C2</f>
+        <v>5.5531358885017222E-2</v>
       </c>
       <c r="R2" s="2">
         <v>3333521.2391999899</v>
+      </c>
+      <c r="S2" s="3">
+        <f>(C2/C$5)*B$5</f>
+        <v>-77.777777777777558</v>
+      </c>
+      <c r="T2" s="3">
+        <f>ABS(B2-S2)</f>
+        <v>18.777777777777658</v>
       </c>
       <c r="X2" s="2">
         <v>5237.99999999999</v>
@@ -4928,28 +4984,34 @@
         <v>55511.999999999898</v>
       </c>
       <c r="D3" s="2">
-        <v>12403.9999999999</v>
+        <f t="shared" ref="D3:D7" si="0">X3/C3</f>
+        <v>0.22344718259115007</v>
       </c>
       <c r="E3" s="2">
         <v>25869.387780000001</v>
       </c>
       <c r="F3" s="2">
-        <v>44881.699999999903</v>
+        <f t="shared" ref="F3:F7" si="1">Z3/C3</f>
+        <v>0.8085044675025217</v>
       </c>
       <c r="G3" s="2">
-        <v>1250.99999999999</v>
+        <f t="shared" ref="G3:G7" si="2">AA3/C3</f>
+        <v>2.2535667963683389E-2</v>
       </c>
       <c r="H3" s="2">
-        <v>2072866.7535099899</v>
+        <f t="shared" ref="H3:H7" si="3">AB3/C3</f>
+        <v>37.340876810599397</v>
       </c>
       <c r="I3" s="2">
         <v>24.21</v>
       </c>
       <c r="J3" s="2">
-        <v>107.99999999999901</v>
+        <f t="shared" ref="J3:J7" si="4">AD3/C3</f>
+        <v>1.9455252918287795E-3</v>
       </c>
       <c r="K3" s="2">
-        <v>173.99999999999901</v>
+        <f t="shared" ref="K3:K7" si="5">AE3/C3</f>
+        <v>3.1344574146130446E-3</v>
       </c>
       <c r="L3" s="2">
         <v>224.39999999999901</v>
@@ -4958,19 +5020,30 @@
         <v>5582.99999999999</v>
       </c>
       <c r="N3" s="2">
-        <v>15403.2</v>
+        <f t="shared" ref="N3:N7" si="6">AH3/C3</f>
+        <v>0.27747514051016048</v>
       </c>
       <c r="O3" s="2">
         <v>200581.14289999899</v>
       </c>
       <c r="P3" s="2">
-        <v>10.999999999999901</v>
+        <f t="shared" ref="P3:P7" si="7">AJ3/C3</f>
+        <v>1.9815535379737572E-4</v>
       </c>
       <c r="Q3" s="2">
-        <v>3031.99999999999</v>
+        <f t="shared" ref="Q3:Q7" si="8">AK3/C3</f>
+        <v>5.4618821155786056E-2</v>
       </c>
       <c r="R3" s="2">
         <v>11707563.6404499</v>
+      </c>
+      <c r="S3" s="3">
+        <f>(C3/C$5)*B$5</f>
+        <v>-188.04878048780481</v>
+      </c>
+      <c r="T3" s="3">
+        <f t="shared" ref="T3:T7" si="9">ABS(B3-S3)</f>
+        <v>57.0487804878058</v>
       </c>
       <c r="X3" s="2">
         <v>12403.9999999999</v>
@@ -5029,28 +5102,34 @@
         <v>171406</v>
       </c>
       <c r="D4" s="2">
-        <v>40166</v>
+        <f t="shared" si="0"/>
+        <v>0.23433252044852573</v>
       </c>
       <c r="E4" s="2">
         <v>26589.534989999898</v>
       </c>
       <c r="F4" s="2">
-        <v>155755.29999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.90869222780999492</v>
       </c>
       <c r="G4" s="2">
-        <v>5458</v>
+        <f t="shared" si="2"/>
+        <v>3.184252593258112E-2</v>
       </c>
       <c r="H4" s="2">
-        <v>9092234.1109599993</v>
+        <f t="shared" si="3"/>
+        <v>53.045016574448965</v>
       </c>
       <c r="I4" s="2">
         <v>24.5</v>
       </c>
       <c r="J4" s="2">
-        <v>288</v>
+        <f t="shared" si="4"/>
+        <v>1.680221229128502E-3</v>
       </c>
       <c r="K4" s="2">
-        <v>615</v>
+        <f t="shared" si="5"/>
+        <v>3.5879724163681553E-3</v>
       </c>
       <c r="L4" s="2">
         <v>404.6</v>
@@ -5059,19 +5138,30 @@
         <v>7062.99999999999</v>
       </c>
       <c r="N4" s="2">
-        <v>44136.1899999999</v>
+        <f t="shared" si="6"/>
+        <v>0.25749501184322543</v>
       </c>
       <c r="O4" s="2">
         <v>398924.45399999898</v>
       </c>
       <c r="P4" s="2">
-        <v>47</v>
+        <f t="shared" si="7"/>
+        <v>2.7420277003138748E-4</v>
       </c>
       <c r="Q4" s="2">
-        <v>8777</v>
+        <f t="shared" si="8"/>
+        <v>5.1205908777989105E-2</v>
       </c>
       <c r="R4" s="2">
         <v>51079825.445459999</v>
+      </c>
+      <c r="S4" s="3">
+        <f>(C4/C$5)*B$5</f>
+        <v>-580.64363143631522</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="9"/>
+        <v>537.64363143631533</v>
       </c>
       <c r="X4" s="2">
         <v>40166</v>
@@ -5130,28 +5220,34 @@
         <v>26567.999999999902</v>
       </c>
       <c r="D5" s="2">
-        <v>4619.99999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.17389340560072294</v>
       </c>
       <c r="E5" s="2">
         <v>20864.893629999999</v>
       </c>
       <c r="F5" s="2">
-        <v>18799.999999999902</v>
+        <f t="shared" si="1"/>
+        <v>0.70761818729298298</v>
       </c>
       <c r="G5" s="2">
-        <v>509.99999999999898</v>
+        <f t="shared" si="2"/>
+        <v>1.9196025293586303E-2</v>
       </c>
       <c r="H5" s="2">
-        <v>723946.50999999896</v>
+        <f t="shared" si="3"/>
+        <v>27.248814739536346</v>
       </c>
       <c r="I5" s="2">
         <v>27.3</v>
       </c>
       <c r="J5" s="2">
-        <v>83</v>
+        <f t="shared" si="4"/>
+        <v>3.1240590183679732E-3</v>
       </c>
       <c r="K5" s="2">
-        <v>62.999999999999901</v>
+        <f t="shared" si="5"/>
+        <v>2.3712737127371325E-3</v>
       </c>
       <c r="L5" s="2">
         <v>376.099999999999</v>
@@ -5160,19 +5256,29 @@
         <v>27861.999999999902</v>
       </c>
       <c r="N5" s="2">
-        <v>17136.699999999899</v>
+        <f t="shared" si="6"/>
+        <v>0.64501279735019434</v>
       </c>
       <c r="O5" s="2">
         <v>785721</v>
       </c>
       <c r="P5" s="2">
-        <v>23.999999999999901</v>
+        <f t="shared" si="7"/>
+        <v>9.0334236675700054E-4</v>
       </c>
       <c r="Q5" s="2">
-        <v>1615.99999999999</v>
+        <f t="shared" si="8"/>
+        <v>6.0825052694971245E-2</v>
       </c>
       <c r="R5" s="2">
         <v>2191476.81674999</v>
+      </c>
+      <c r="S5" s="3">
+        <v>-89.999999999999801</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="X5" s="2">
         <v>4619.99999999999</v>
@@ -5231,28 +5337,34 @@
         <v>58750.999999999898</v>
       </c>
       <c r="D6" s="2">
-        <v>16366.4999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.27857398171945885</v>
       </c>
       <c r="E6" s="2">
         <v>41719.813269999999</v>
       </c>
       <c r="F6" s="2">
-        <v>51864.3999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.88278327177409732</v>
       </c>
       <c r="G6" s="2">
-        <v>1966.99999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.3480281186703091E-2</v>
       </c>
       <c r="H6" s="2">
-        <v>2778929.7944199899</v>
+        <f t="shared" si="3"/>
+        <v>47.300127562424379</v>
       </c>
       <c r="I6" s="2">
         <v>24.8</v>
       </c>
       <c r="J6" s="2">
-        <v>112.99999999999901</v>
+        <f t="shared" si="4"/>
+        <v>1.9233715170805467E-3</v>
       </c>
       <c r="K6" s="2">
-        <v>187.49999999999901</v>
+        <f t="shared" si="5"/>
+        <v>3.1914350394035731E-3</v>
       </c>
       <c r="L6" s="2">
         <v>113.599999999999</v>
@@ -5261,19 +5373,30 @@
         <v>1522.49999999999</v>
       </c>
       <c r="N6" s="2">
-        <v>9524.6999999999898</v>
+        <f t="shared" si="6"/>
+        <v>0.16211979370563917</v>
       </c>
       <c r="O6" s="2">
         <v>133992.89939999901</v>
       </c>
       <c r="P6" s="2">
-        <v>10.999999999999901</v>
+        <f t="shared" si="7"/>
+        <v>1.8723085564500893E-4</v>
       </c>
       <c r="Q6" s="2">
-        <v>3699.49999999999</v>
+        <f t="shared" si="8"/>
+        <v>6.2969140950792271E-2</v>
       </c>
       <c r="R6" s="2">
         <v>59607023.156849898</v>
+      </c>
+      <c r="S6" s="3">
+        <f>(C6/C$5)*B$5</f>
+        <v>-199.02100271002703</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" si="9"/>
+        <v>64.021002710028029</v>
       </c>
       <c r="X6" s="2">
         <v>16366.4999999999</v>
@@ -5332,28 +5455,34 @@
         <v>105040.5</v>
       </c>
       <c r="D7" s="2">
-        <v>24045.999999999902</v>
+        <f t="shared" si="0"/>
+        <v>0.22892122562249706</v>
       </c>
       <c r="E7" s="2">
         <v>23627.867339999899</v>
       </c>
       <c r="F7" s="2">
-        <v>90214.099999999904</v>
+        <f t="shared" si="1"/>
+        <v>0.85885063380315119</v>
       </c>
       <c r="G7" s="2">
-        <v>2856.5</v>
+        <f t="shared" si="2"/>
+        <v>2.7194272685297574E-2</v>
       </c>
       <c r="H7" s="2">
-        <v>4988641.7706300002</v>
+        <f t="shared" si="3"/>
+        <v>47.492555448898287</v>
       </c>
       <c r="I7" s="2">
         <v>24.9</v>
       </c>
       <c r="J7" s="2">
-        <v>188.49999999999901</v>
+        <f t="shared" si="4"/>
+        <v>1.7945459132429778E-3</v>
       </c>
       <c r="K7" s="2">
-        <v>284</v>
+        <f t="shared" si="5"/>
+        <v>2.7037190417029621E-3</v>
       </c>
       <c r="L7" s="2">
         <v>241.74999999999901</v>
@@ -5362,19 +5491,30 @@
         <v>4924.49999999999</v>
       </c>
       <c r="N7" s="2">
-        <v>23106.964999999898</v>
+        <f t="shared" si="6"/>
+        <v>0.21998148333261835</v>
       </c>
       <c r="O7" s="2">
         <v>206293.05819999901</v>
       </c>
       <c r="P7" s="2">
-        <v>28.999999999999901</v>
+        <f t="shared" si="7"/>
+        <v>2.7608398665276632E-4</v>
       </c>
       <c r="Q7" s="2">
-        <v>5729.49999999999</v>
+        <f t="shared" si="8"/>
+        <v>5.454562763886301E-2</v>
       </c>
       <c r="R7" s="2">
         <v>19580455.535099901</v>
+      </c>
+      <c r="S7" s="3">
+        <f>(C7/C$5)*B$5</f>
+        <v>-355.82825203252088</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="9"/>
+        <v>259.32825203252099</v>
       </c>
       <c r="X7" s="2">
         <v>24045.999999999902</v>
@@ -5424,6 +5564,186 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C7">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D7">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E7">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F7">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G7">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H7">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I7">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J7">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L7">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M7">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N7">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P7">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q7">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R7">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5435,7 +5755,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="T2:T7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5448,6 +5768,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New criteria for clusters
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/median of clusters (no mundist-f).xlsx
+++ b/migforecasting/clustering/median of clusters (no mundist-f).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>clust</t>
   </si>
@@ -98,12 +98,15 @@
   <si>
     <t>wors case</t>
   </si>
+  <si>
+    <t>Mig prop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +125,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -188,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -213,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4766,8 +4784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4777,7 +4795,7 @@
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" customWidth="1"/>
     <col min="21" max="21" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4836,10 +4854,13 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="X1" s="1" t="s">
@@ -4952,12 +4973,16 @@
       <c r="R2" s="5">
         <v>3333521.2391999899</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="10">
+        <f>B2/C2</f>
+        <v>-2.5696864111498323E-3</v>
+      </c>
+      <c r="T2" s="3">
         <f>(C2/C$5)*B$5</f>
         <v>-77.777777777777558</v>
       </c>
-      <c r="T2" s="3">
-        <f>ABS(B2-S2)</f>
+      <c r="U2" s="3">
+        <f t="shared" ref="U2:U7" si="0">ABS(B2-T2)</f>
         <v>18.777777777777658</v>
       </c>
       <c r="X2" s="2">
@@ -5017,33 +5042,33 @@
         <v>55511.999999999898</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D7" si="0">X3/C3</f>
+        <f t="shared" ref="D3:D7" si="1">X3/C3</f>
         <v>0.22344718259115007</v>
       </c>
       <c r="E3" s="2">
         <v>25869.387780000001</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F7" si="1">Z3/C3</f>
+        <f t="shared" ref="F3:F7" si="2">Z3/C3</f>
         <v>0.8085044675025217</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G7" si="2">AA3/C3</f>
+        <f t="shared" ref="G3:G7" si="3">AA3/C3</f>
         <v>2.2535667963683389E-2</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H7" si="3">AB3/C3</f>
+        <f t="shared" ref="H3:H7" si="4">AB3/C3</f>
         <v>37.340876810599397</v>
       </c>
       <c r="I3" s="2">
         <v>24.21</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J7" si="4">AD3/C3</f>
+        <f t="shared" ref="J3:J7" si="5">AD3/C3</f>
         <v>1.9455252918287795E-3</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K7" si="5">AE3/C3</f>
+        <f t="shared" ref="K3:K7" si="6">AE3/C3</f>
         <v>3.1344574146130446E-3</v>
       </c>
       <c r="L3" s="2">
@@ -5053,29 +5078,33 @@
         <v>5582.99999999999</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" ref="N3:N7" si="6">AH3/C3</f>
+        <f t="shared" ref="N3:N7" si="7">AH3/C3</f>
         <v>0.27747514051016048</v>
       </c>
       <c r="O3" s="2">
         <v>200581.14289999899</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" ref="P3:P7" si="7">AJ3/C3</f>
+        <f t="shared" ref="P3:P7" si="8">AJ3/C3</f>
         <v>1.9815535379737572E-4</v>
       </c>
       <c r="Q3" s="2">
-        <f t="shared" ref="Q3:Q7" si="8">AK3/C3</f>
+        <f t="shared" ref="Q3:Q7" si="9">AK3/C3</f>
         <v>5.4618821155786056E-2</v>
       </c>
       <c r="R3" s="5">
         <v>11707563.6404499</v>
       </c>
-      <c r="S3" s="3">
+      <c r="S3" s="10">
+        <f t="shared" ref="S3:S7" si="10">B3/C3</f>
+        <v>-2.3598501224960234E-3</v>
+      </c>
+      <c r="T3" s="3">
         <f>(C3/C$5)*B$5</f>
         <v>-188.04878048780481</v>
       </c>
-      <c r="T3" s="3">
-        <f t="shared" ref="T3:T7" si="9">ABS(B3-S3)</f>
+      <c r="U3" s="3">
+        <f t="shared" si="0"/>
         <v>57.0487804878058</v>
       </c>
       <c r="X3" s="2">
@@ -5135,33 +5164,33 @@
         <v>171406</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23433252044852573</v>
       </c>
       <c r="E4" s="2">
         <v>26589.534989999898</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90869222780999492</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.184252593258112E-2</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53.045016574448965</v>
       </c>
       <c r="I4" s="2">
         <v>24.5</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.680221229128502E-3</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5879724163681553E-3</v>
       </c>
       <c r="L4" s="2">
@@ -5171,29 +5200,33 @@
         <v>7062.99999999999</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.25749501184322543</v>
       </c>
       <c r="O4" s="2">
         <v>398924.45399999898</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.7420277003138748E-4</v>
       </c>
       <c r="Q4" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.1205908777989105E-2</v>
       </c>
       <c r="R4" s="5">
         <v>51079825.445459999</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="10">
+        <f t="shared" si="10"/>
+        <v>-2.5086636407126883E-4</v>
+      </c>
+      <c r="T4" s="3">
         <f>(C4/C$5)*B$5</f>
         <v>-580.64363143631522</v>
       </c>
-      <c r="T4" s="3">
-        <f t="shared" si="9"/>
+      <c r="U4" s="3">
+        <f t="shared" si="0"/>
         <v>537.64363143631533</v>
       </c>
       <c r="X4" s="2">
@@ -5253,33 +5286,33 @@
         <v>26567.999999999902</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17389340560072294</v>
       </c>
       <c r="E5" s="2">
         <v>20864.893629999999</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.70761818729298298</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9196025293586303E-2</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27.248814739536346</v>
       </c>
       <c r="I5" s="2">
         <v>27.3</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1240590183679732E-3</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.3712737127371325E-3</v>
       </c>
       <c r="L5" s="2">
@@ -5289,28 +5322,32 @@
         <v>27861.999999999902</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.64501279735019434</v>
       </c>
       <c r="O5" s="2">
         <v>785721</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.0334236675700054E-4</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0825052694971245E-2</v>
       </c>
       <c r="R5" s="5">
         <v>2191476.81674999</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="10">
+        <f t="shared" si="10"/>
+        <v>-3.3875338753387584E-3</v>
+      </c>
+      <c r="T5" s="3">
         <v>-89.999999999999801</v>
       </c>
-      <c r="T5" s="3">
-        <f t="shared" si="9"/>
+      <c r="U5" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X5" s="2">
@@ -5370,33 +5407,33 @@
         <v>58750.999999999898</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.27857398171945885</v>
       </c>
       <c r="E6" s="2">
         <v>41719.813269999999</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88278327177409732</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3480281186703091E-2</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.300127562424379</v>
       </c>
       <c r="I6" s="2">
         <v>24.8</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9233715170805467E-3</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1914350394035731E-3</v>
       </c>
       <c r="L6" s="2">
@@ -5406,29 +5443,33 @@
         <v>1522.49999999999</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.16211979370563917</v>
       </c>
       <c r="O6" s="2">
         <v>133992.89939999901</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8723085564500893E-4</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2969140950792271E-2</v>
       </c>
       <c r="R6" s="5">
         <v>59607023.156849898</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="10">
+        <f t="shared" si="10"/>
+        <v>-2.2978332283705681E-3</v>
+      </c>
+      <c r="T6" s="3">
         <f>(C6/C$5)*B$5</f>
         <v>-199.02100271002703</v>
       </c>
-      <c r="T6" s="3">
-        <f t="shared" si="9"/>
+      <c r="U6" s="3">
+        <f t="shared" si="0"/>
         <v>64.021002710028029</v>
       </c>
       <c r="X6" s="2">
@@ -5488,33 +5529,33 @@
         <v>105040.5</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.22892122562249706</v>
       </c>
       <c r="E7" s="2">
         <v>23627.867339999899</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85885063380315119</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7194272685297574E-2</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.492555448898287</v>
       </c>
       <c r="I7" s="2">
         <v>24.9</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7945459132429778E-3</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.7037190417029621E-3</v>
       </c>
       <c r="L7" s="2">
@@ -5524,29 +5565,33 @@
         <v>4924.49999999999</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.21998148333261835</v>
       </c>
       <c r="O7" s="2">
         <v>206293.05819999901</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.7608398665276632E-4</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.454562763886301E-2</v>
       </c>
       <c r="R7" s="5">
         <v>19580455.535099901</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="10">
+        <f t="shared" si="10"/>
+        <v>-9.1869326593075912E-4</v>
+      </c>
+      <c r="T7" s="3">
         <f>(C7/C$5)*B$5</f>
         <v>-355.82825203252088</v>
       </c>
-      <c r="T7" s="3">
-        <f t="shared" si="9"/>
+      <c r="U7" s="3">
+        <f t="shared" si="0"/>
         <v>259.32825203252099</v>
       </c>
       <c r="X7" s="2">
@@ -5597,6 +5642,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C7">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -5608,7 +5665,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="E2:E7">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -5620,7 +5677,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E7">
+  <conditionalFormatting sqref="F2:F7">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -5632,7 +5689,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F7">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -5644,7 +5701,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -5656,7 +5713,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -5668,7 +5725,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -5680,7 +5737,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="K2:K7">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -5692,7 +5749,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K7">
+  <conditionalFormatting sqref="L2:L7">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -5704,7 +5761,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L7">
+  <conditionalFormatting sqref="M2:M7">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -5716,7 +5773,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M7">
+  <conditionalFormatting sqref="N2:N7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -5728,7 +5785,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N7">
+  <conditionalFormatting sqref="O2:O7">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -5740,7 +5797,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O7">
+  <conditionalFormatting sqref="P2:P7">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -5752,7 +5809,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P7">
+  <conditionalFormatting sqref="Q2:Q7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -5764,7 +5821,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q7">
+  <conditionalFormatting sqref="R2:R7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5776,7 +5833,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R7">
+  <conditionalFormatting sqref="U2:U7">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5788,7 +5845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T7">
+  <conditionalFormatting sqref="S2:S7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>